<commit_message>
Import data from list supports importing references, not just plain properties
</commit_message>
<xml_diff>
--- a/OpenXavaTest/test-files/appointments.xlsx
+++ b/OpenXavaTest/test-files/appointments.xlsx
@@ -5,43 +5,60 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="appointments" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Some comments</t>
-  </si>
-  <si>
-    <t>Amount of people</t>
-  </si>
-  <si>
-    <t>Start time</t>
-  </si>
-  <si>
-    <t>Descrip</t>
-  </si>
-  <si>
-    <t>Meeting with my friend</t>
-  </si>
-  <si>
-    <t>NAP</t>
-  </si>
-  <si>
-    <t>As fast as possible</t>
-  </si>
-  <si>
-    <t>Driving my BMW</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t xml:space="preserve">Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Some comments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount of people</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descrip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type of type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level of type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting with my friend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As fast as possible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driving my BMW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Playing Fortnite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
   </si>
 </sst>
 </file>
@@ -49,7 +66,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M/D/YY\ H:MM\ AM/PM"/>
   </numFmts>
   <fonts count="5">
@@ -139,12 +156,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -154,19 +171,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="30.3214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="30.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.4285714285714"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="30.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -185,6 +202,12 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
@@ -197,7 +220,7 @@
         <v>42989.4895833333</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -205,7 +228,7 @@
         <v>42990.6666666667</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="2" t="n">
@@ -217,20 +240,40 @@
         <v>42991.8125</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="2" t="n">
         <v>42991.8333333333</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
+        <v>44001.8541666667</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>44001.84375</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>